<commit_message>
rename image file extensions
</commit_message>
<xml_diff>
--- a/documents/o2conc.xlsx
+++ b/documents/o2conc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickos01/Desktop/O24U/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mickos01/Desktop/O24U/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E230FDD-5D7E-C949-B4BF-A2073ED2EB76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DA8848-7C80-2940-BFDF-D67B265100FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="500" windowWidth="25120" windowHeight="16820" tabRatio="500" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2560" yWindow="500" windowWidth="25120" windowHeight="16820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Volume" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="704">
   <si>
     <t>liters</t>
   </si>
@@ -2149,6 +2149,9 @@
   </si>
   <si>
     <t>Consumable</t>
+  </si>
+  <si>
+    <t>JLOX-101 data sheet</t>
   </si>
 </sst>
 </file>
@@ -2810,10 +2813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2821,6 +2824,14 @@
     <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:13">
+      <c r="H1">
+        <v>0.63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>703</v>
+      </c>
+    </row>
     <row r="2" spans="1:13">
       <c r="H2">
         <v>0.64</v>
@@ -2842,7 +2853,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="F4">
-        <v>0.79</v>
+        <v>0.63</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -2901,18 +2912,24 @@
       </c>
       <c r="G6" s="27">
         <f>E6*F$4</f>
-        <v>2.0937360203661441</v>
+        <v>1.6696882187730009</v>
       </c>
       <c r="H6" s="28">
         <f>F6*G6</f>
-        <v>4.1874720407322883</v>
+        <v>3.3393764375460018</v>
       </c>
       <c r="I6" s="28">
         <f>H6*2.2</f>
-        <v>9.212438489611035</v>
+        <v>7.3466281626012044</v>
       </c>
       <c r="J6" t="s">
         <v>376</v>
+      </c>
+      <c r="L6">
+        <v>2.5</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2939,18 +2956,26 @@
       </c>
       <c r="G7" s="27">
         <f>E7*F$4</f>
-        <v>1.5912393754782694</v>
+        <v>1.2689630462674806</v>
       </c>
       <c r="H7" s="28">
         <f>F7*G7</f>
-        <v>3.1824787509565389</v>
+        <v>2.5379260925349612</v>
       </c>
       <c r="I7" s="28">
         <f>H7*2.2</f>
-        <v>7.001453252104386</v>
+        <v>5.583437403576915</v>
       </c>
       <c r="J7" t="s">
         <v>377</v>
+      </c>
+      <c r="L7" s="1">
+        <f>H6/L6</f>
+        <v>1.3357505750184007</v>
+      </c>
+      <c r="M7" s="1">
+        <f>M6*L7</f>
+        <v>13.357505750184007</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2977,15 +3002,15 @@
       </c>
       <c r="G9" s="2">
         <f t="shared" ref="G9:G15" si="2">E9*F$4</f>
-        <v>0.89077869222581141</v>
+        <v>0.71036781785096348</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" ref="H9" si="3">F9*G9</f>
-        <v>0.89077869222581141</v>
+        <v>0.71036781785096348</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" ref="I9:I15" si="4">H9*2.2</f>
-        <v>1.9597131228967852</v>
+        <v>1.5628091992721198</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -3012,15 +3037,15 @@
       </c>
       <c r="G10" s="2">
         <f t="shared" si="2"/>
-        <v>0.67699180609161669</v>
+        <v>0.53987954156673235</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" ref="H10" si="5">F10*G10</f>
-        <v>0.67699180609161669</v>
+        <v>0.53987954156673235</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="4"/>
-        <v>1.4893819734015568</v>
+        <v>1.1877349914468112</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -3047,15 +3072,15 @@
       </c>
       <c r="G11" s="2">
         <f t="shared" si="2"/>
-        <v>0.46320491995742197</v>
+        <v>0.36939126528250105</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" ref="H11" si="6">F11*G11</f>
-        <v>0.46320491995742197</v>
+        <v>0.36939126528250105</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="4"/>
-        <v>1.0190508239063285</v>
+        <v>0.8126607836215024</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -3082,15 +3107,15 @@
       </c>
       <c r="G12" s="2">
         <f t="shared" si="2"/>
-        <v>0.70609149585466857</v>
+        <v>0.5630856232765078</v>
       </c>
       <c r="H12" s="1">
         <f>F12*G12</f>
-        <v>0.70609149585466857</v>
+        <v>0.5630856232765078</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="4"/>
-        <v>1.553401290880271</v>
+        <v>1.2387883712083172</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -3117,15 +3142,15 @@
       </c>
       <c r="G13" s="27">
         <f t="shared" si="2"/>
-        <v>0.47708884855045164</v>
+        <v>0.38046325897061328</v>
       </c>
       <c r="H13" s="28">
         <f t="shared" ref="H13" si="7">F13*G13</f>
-        <v>0.47708884855045164</v>
+        <v>0.38046325897061328</v>
       </c>
       <c r="I13" s="28">
         <f t="shared" si="4"/>
-        <v>1.0495954668109937</v>
+        <v>0.83701916973534929</v>
       </c>
       <c r="J13" t="s">
         <v>378</v>
@@ -3155,15 +3180,15 @@
       </c>
       <c r="G14" s="2">
         <f t="shared" si="2"/>
-        <v>0.36258752489834328</v>
+        <v>0.28915207681766614</v>
       </c>
       <c r="H14" s="1">
         <f>F14*G14</f>
-        <v>0.36258752489834328</v>
+        <v>0.28915207681766614</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="4"/>
-        <v>0.79769255477635526</v>
+        <v>0.63613456899886556</v>
       </c>
       <c r="K14">
         <f>A14*25.4</f>
@@ -3201,15 +3226,15 @@
       </c>
       <c r="G15" s="27">
         <f t="shared" si="2"/>
-        <v>0.17175198547816259</v>
+        <v>0.1369667732294208</v>
       </c>
       <c r="H15" s="28">
         <f t="shared" ref="H15" si="8">F15*G15</f>
-        <v>0.17175198547816259</v>
+        <v>0.1369667732294208</v>
       </c>
       <c r="I15" s="28">
         <f t="shared" si="4"/>
-        <v>0.37785436805195771</v>
+        <v>0.30132690110472576</v>
       </c>
       <c r="J15" t="s">
         <v>379</v>
@@ -3247,15 +3272,15 @@
       </c>
       <c r="G17" s="2">
         <f>E17*F$4</f>
-        <v>1.1547232871442537</v>
+        <v>0.92085527962136671</v>
       </c>
       <c r="H17" s="1">
         <f>F17*G17</f>
-        <v>2.3094465742885073</v>
+        <v>1.8417105592427334</v>
       </c>
       <c r="I17" s="1">
         <f>H17*2.2</f>
-        <v>5.0807824634347165</v>
+        <v>4.0517632303340134</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -3282,15 +3307,15 @@
       </c>
       <c r="G18" s="27">
         <f>E18*F$4</f>
-        <v>1.2701956158586793</v>
+        <v>1.0129408075835038</v>
       </c>
       <c r="H18" s="28">
         <f>F18*G18</f>
-        <v>1.2701956158586793</v>
+        <v>1.0129408075835038</v>
       </c>
       <c r="I18" s="28">
         <f>H18*2.2</f>
-        <v>2.7944303548890947</v>
+        <v>2.2284697766837085</v>
       </c>
       <c r="J18" t="s">
         <v>374</v>
@@ -3326,15 +3351,15 @@
       </c>
       <c r="G19" s="2">
         <f>E19*F$4</f>
-        <v>2.3094465742885073</v>
+        <v>1.8417105592427334</v>
       </c>
       <c r="H19" s="1">
         <f>F19*G19</f>
-        <v>4.6188931485770146</v>
+        <v>3.6834211184854668</v>
       </c>
       <c r="I19" s="1">
         <f>H19*2.2</f>
-        <v>10.161564926869433</v>
+        <v>8.1035264606680268</v>
       </c>
       <c r="L19" s="2">
         <f>L18/L14*L16</f>
@@ -3368,15 +3393,15 @@
       </c>
       <c r="G20" s="27">
         <f>E20*F$4</f>
-        <v>2.4249189030029332</v>
+        <v>1.9337960872048705</v>
       </c>
       <c r="H20" s="28">
         <f>F20*G20</f>
-        <v>2.4249189030029332</v>
+        <v>1.9337960872048705</v>
       </c>
       <c r="I20" s="28">
         <f>H20*2.2</f>
-        <v>5.3348215866064539</v>
+        <v>4.2543513918507152</v>
       </c>
       <c r="J20" t="s">
         <v>375</v>
@@ -3406,15 +3431,15 @@
       </c>
       <c r="G21" s="2">
         <f>E21*F$4</f>
-        <v>2.7410222295358233</v>
+        <v>2.1858784868450236</v>
       </c>
       <c r="H21" s="1">
         <f>F21*G21</f>
-        <v>2.7410222295358233</v>
+        <v>2.1858784868450236</v>
       </c>
       <c r="I21" s="1">
         <f>H21*2.2</f>
-        <v>6.0302489049788122</v>
+        <v>4.8089326710590523</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -3461,15 +3486,15 @@
       </c>
       <c r="G24" s="2">
         <f>E24*F$4</f>
-        <v>2.0450081597484262</v>
+        <v>1.6308292919512763</v>
       </c>
       <c r="H24" s="1">
         <f>F24*G24</f>
-        <v>4.0900163194968524</v>
+        <v>3.2616585839025527</v>
       </c>
       <c r="I24" s="1">
         <f>H24*2.2</f>
-        <v>8.9980359028930756</v>
+        <v>7.1756488845856161</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -3552,7 +3577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>